<commit_message>
implimented regression modeling and mixed effect regression modeling; changed figures
</commit_message>
<xml_diff>
--- a/annotation/virus_genome_taxaControlled_motif.xlsx
+++ b/annotation/virus_genome_taxaControlled_motif.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">Estimate</t>
   </si>
@@ -44,6 +44,9 @@
     <t xml:space="preserve">motif</t>
   </si>
   <si>
+    <t xml:space="preserve">var</t>
+  </si>
+  <si>
     <t xml:space="preserve">none</t>
   </si>
   <si>
@@ -53,6 +56,12 @@
     <t xml:space="preserve">G00065MO</t>
   </si>
   <si>
+    <t xml:space="preserve">ss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ds</t>
+  </si>
+  <si>
     <t xml:space="preserve">genus</t>
   </si>
   <si>
@@ -104,7 +113,13 @@
     <t xml:space="preserve">G00046MO</t>
   </si>
   <si>
-    <t xml:space="preserve">strand_X</t>
+    <t xml:space="preserve">neg_pos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">neg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos</t>
   </si>
 </sst>
 </file>
@@ -467,6 +482,9 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -486,14 +504,17 @@
         <v>94.9198004193363</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H2"/>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -514,14 +535,17 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H3"/>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -544,16 +568,19 @@
         <v>-11.8653142316683</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H4" t="n">
         <v>0.203571391102523</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -576,16 +603,19 @@
         <v>#NUM!</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H5" t="n">
         <v>0.203571391102523</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J5" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -606,13 +636,16 @@
         <v>94.9197997461972</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H6"/>
       <c r="I6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -634,14 +667,17 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H7"/>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J7" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8">
@@ -662,14 +698,17 @@
         <v>284.483932456264</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H8"/>
       <c r="I8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J8" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -690,13 +729,16 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H9"/>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -720,16 +762,19 @@
         <v>#NUM!</v>
       </c>
       <c r="G10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H10" t="n">
         <v>0.851658199230797</v>
       </c>
       <c r="I10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J10" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="K10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11">
@@ -752,15 +797,18 @@
         <v>#NUM!</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H11" t="n">
         <v>0.851658199230797</v>
       </c>
       <c r="I11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -784,14 +832,17 @@
         <v>0.524695620139675</v>
       </c>
       <c r="G12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H12"/>
       <c r="I12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13">
@@ -814,14 +865,17 @@
         <v>2.3795591936803</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H13"/>
       <c r="I13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J13" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14">
@@ -844,16 +898,19 @@
         <v>30.3574535064021</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H14" t="n">
         <v>0.439803846377566</v>
       </c>
       <c r="I14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K14" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15">
@@ -876,16 +933,19 @@
         <v>20.5875161585311</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H15" t="n">
         <v>0.439803846377566</v>
       </c>
       <c r="I15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J15" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16">
@@ -908,14 +968,17 @@
         <v>0.52469562013967</v>
       </c>
       <c r="G16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="K16" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -938,14 +1001,17 @@
         <v>5.29709038871112</v>
       </c>
       <c r="G17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H17"/>
       <c r="I17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J17" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="K17" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18">
@@ -968,16 +1034,19 @@
         <v>1.60301198505774</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H18" t="n">
         <v>0.226721917750159</v>
       </c>
       <c r="I18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J18" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="K18" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19">
@@ -1000,16 +1069,19 @@
         <v>5.98600822529888</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H19" t="n">
         <v>0.226721917750159</v>
       </c>
       <c r="I19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="K19" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20">
@@ -1030,14 +1102,17 @@
         <v>480.078912560535</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H20"/>
       <c r="I20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J20" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="K20" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="21">
@@ -1058,14 +1133,17 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H21"/>
       <c r="I21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J21" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="K21" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22">
@@ -1088,16 +1166,19 @@
         <v>#NUM!</v>
       </c>
       <c r="G22" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H22" t="n">
         <v>0.793533261135444</v>
       </c>
       <c r="I22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J22" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="K22" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23">
@@ -1120,16 +1201,19 @@
         <v>#NUM!</v>
       </c>
       <c r="G23" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H23" t="n">
         <v>0.793533261135444</v>
       </c>
       <c r="I23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J23" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="K23" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="24">
@@ -1150,14 +1234,17 @@
         <v>480.078912560535</v>
       </c>
       <c r="G24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H24"/>
       <c r="I24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J24" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="K24" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="25">
@@ -1178,14 +1265,17 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H25"/>
       <c r="I25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J25" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="K25" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="26">
@@ -1208,16 +1298,19 @@
         <v>#NUM!</v>
       </c>
       <c r="G26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H26" t="n">
         <v>0.793533261135444</v>
       </c>
       <c r="I26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J26" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="K26" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="27">
@@ -1240,16 +1333,19 @@
         <v>#NUM!</v>
       </c>
       <c r="G27" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H27" t="n">
         <v>0.793533261135444</v>
       </c>
       <c r="I27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J27" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="K27" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="28">
@@ -1270,14 +1366,17 @@
         <v>94.9197994793382</v>
       </c>
       <c r="G28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H28"/>
       <c r="I28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J28" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="K28" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="29">
@@ -1298,14 +1397,17 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H29"/>
       <c r="I29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J29" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="K29" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="30">
@@ -1328,14 +1430,17 @@
         <v>2.43259636708588</v>
       </c>
       <c r="G30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H30"/>
       <c r="I30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J30" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="K30" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="31">
@@ -1358,14 +1463,17 @@
         <v>-1.44659775751298</v>
       </c>
       <c r="G31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H31"/>
       <c r="I31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J31" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="K31" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="32">
@@ -1388,16 +1496,19 @@
         <v>3.48820096957888</v>
       </c>
       <c r="G32" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H32" t="n">
         <v>0.0380565651809334</v>
       </c>
       <c r="I32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J32" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="K32" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="33">
@@ -1420,16 +1531,19 @@
         <v>-0.297269879270204</v>
       </c>
       <c r="G33" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H33" t="n">
         <v>0.0380565651809334</v>
       </c>
       <c r="I33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J33" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="K33" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="34">
@@ -1452,14 +1566,17 @@
         <v>0.524695619526974</v>
       </c>
       <c r="G34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H34"/>
       <c r="I34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J34" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="K34" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="35">
@@ -1482,14 +1599,17 @@
         <v>1.70514545155774</v>
       </c>
       <c r="G35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H35"/>
       <c r="I35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J35" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="K35" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="36">
@@ -1512,16 +1632,19 @@
         <v>17.1124510440174</v>
       </c>
       <c r="G36" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H36" t="n">
         <v>0.437325773618966</v>
       </c>
       <c r="I36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J36" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="K36" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="37">
@@ -1544,16 +1667,19 @@
         <v>9.31399544169485</v>
       </c>
       <c r="G37" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H37" t="n">
         <v>0.437325773618966</v>
       </c>
       <c r="I37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J37" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="K37" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="38">
@@ -1574,14 +1700,17 @@
         <v>94.9198001049868</v>
       </c>
       <c r="G38" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H38"/>
       <c r="I38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J38" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="K38" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="39">
@@ -1602,14 +1731,17 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H39"/>
       <c r="I39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J39" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="K39" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="40">
@@ -1630,14 +1762,17 @@
         <v>94.919800128676</v>
       </c>
       <c r="G40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H40"/>
       <c r="I40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J40" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="K40" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="41">
@@ -1658,14 +1793,17 @@
       </c>
       <c r="F41"/>
       <c r="G41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H41"/>
       <c r="I41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J41" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="K41" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="42">
@@ -1686,14 +1824,17 @@
         <v>166.243049805564</v>
       </c>
       <c r="G42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H42"/>
       <c r="I42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J42" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="K42" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="43">
@@ -1714,14 +1855,17 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H43"/>
       <c r="I43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J43" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="K43" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="44">
@@ -1744,14 +1888,17 @@
         <v>2.43259636708588</v>
       </c>
       <c r="G44" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H44"/>
       <c r="I44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J44" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="K44" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="45">
@@ -1774,14 +1921,17 @@
         <v>-1.44659775751298</v>
       </c>
       <c r="G45" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H45"/>
       <c r="I45" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J45" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="K45" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="46">
@@ -1804,16 +1954,19 @@
         <v>3.48820096957888</v>
       </c>
       <c r="G46" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H46" t="n">
         <v>0.0380565651809334</v>
       </c>
       <c r="I46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J46" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="K46" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="47">
@@ -1836,16 +1989,19 @@
         <v>-0.297269879270204</v>
       </c>
       <c r="G47" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H47" t="n">
         <v>0.0380565651809334</v>
       </c>
       <c r="I47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J47" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="K47" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="48">
@@ -1866,14 +2022,17 @@
         <v>166.24305026445</v>
       </c>
       <c r="G48" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H48"/>
       <c r="I48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J48" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="K48" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="49">
@@ -1894,14 +2053,17 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H49"/>
       <c r="I49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J49" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="K49" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="50">
@@ -1922,14 +2084,17 @@
         <v>166.243050007765</v>
       </c>
       <c r="G50" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H50"/>
       <c r="I50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J50" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="K50" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="51">
@@ -1950,14 +2115,17 @@
       </c>
       <c r="F51"/>
       <c r="G51" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H51"/>
       <c r="I51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J51" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="K51" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="52">
@@ -1978,14 +2146,17 @@
         <v>166.2430516909</v>
       </c>
       <c r="G52" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H52"/>
       <c r="I52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J52" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="K52" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="53">
@@ -2006,14 +2177,17 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H53"/>
       <c r="I53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J53" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="K53" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="54">
@@ -2036,14 +2210,17 @@
         <v>1.15032870110985</v>
       </c>
       <c r="G54" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H54"/>
       <c r="I54" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J54" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K54" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="55">
@@ -2064,14 +2241,17 @@
         <v>38.0458227975472</v>
       </c>
       <c r="G55" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H55"/>
       <c r="I55" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J55" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K55" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="56">
@@ -2094,14 +2274,17 @@
         <v>0.414447170251229</v>
       </c>
       <c r="G56" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H56"/>
       <c r="I56" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J56" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="K56" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="57">
@@ -2122,14 +2305,17 @@
         <v>38.7488406595246</v>
       </c>
       <c r="G57" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H57"/>
       <c r="I57" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J57" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="K57" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="58">
@@ -2152,14 +2338,17 @@
         <v>-89.4737727970003</v>
       </c>
       <c r="G58" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H58"/>
       <c r="I58" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J58" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="K58" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="59">
@@ -2180,14 +2369,17 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H59"/>
       <c r="I59" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J59" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="K59" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="60">
@@ -2210,14 +2402,17 @@
         <v>-134.526945053643</v>
       </c>
       <c r="G60" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H60"/>
       <c r="I60" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J60" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K60" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="61">
@@ -2238,14 +2433,17 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H61"/>
       <c r="I61" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J61" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K61" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="62">
@@ -2268,14 +2466,17 @@
         <v>1.74392500663523</v>
       </c>
       <c r="G62" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H62"/>
       <c r="I62" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J62" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="K62" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="63">
@@ -2298,14 +2499,17 @@
         <v>-1.44003793845995</v>
       </c>
       <c r="G63" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H63"/>
       <c r="I63" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J63" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="K63" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="64">
@@ -2328,14 +2532,17 @@
         <v>-3.33321178768647</v>
       </c>
       <c r="G64" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H64"/>
       <c r="I64" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J64" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="K64" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="65">
@@ -2356,14 +2563,17 @@
         <v>879.96716138172</v>
       </c>
       <c r="G65" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H65"/>
       <c r="I65" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J65" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="K65" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="66">
@@ -2386,14 +2596,17 @@
         <v>-3.33321178768647</v>
       </c>
       <c r="G66" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H66"/>
       <c r="I66" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J66" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="K66" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="67">
@@ -2414,14 +2627,17 @@
         <v>879.96716138172</v>
       </c>
       <c r="G67" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H67"/>
       <c r="I67" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J67" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="K67" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="68">
@@ -2444,14 +2660,17 @@
         <v>0.414447131077413</v>
       </c>
       <c r="G68" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H68"/>
       <c r="I68" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J68" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="K68" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="69">
@@ -2474,14 +2693,17 @@
         <v>-0.229923234721227</v>
       </c>
       <c r="G69" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H69"/>
       <c r="I69" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J69" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="K69" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="70">
@@ -2504,14 +2726,17 @@
         <v>-2.14656976547731</v>
       </c>
       <c r="G70" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H70"/>
       <c r="I70" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J70" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="K70" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="71">
@@ -2532,14 +2757,17 @@
         <v>129.151953893201</v>
       </c>
       <c r="G71" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H71"/>
       <c r="I71" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J71" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="K71" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="72">
@@ -2562,14 +2790,17 @@
         <v>-89.4737727393235</v>
       </c>
       <c r="G72" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H72"/>
       <c r="I72" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J72" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="K72" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="73">
@@ -2590,14 +2821,17 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H73"/>
       <c r="I73" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J73" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="K73" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="74">
@@ -2620,14 +2854,17 @@
         <v>-1.11415010045256</v>
       </c>
       <c r="G74" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H74"/>
       <c r="I74" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J74" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="K74" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="75">
@@ -2648,14 +2885,17 @@
         <v>75.0752921768876</v>
       </c>
       <c r="G75" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H75"/>
       <c r="I75" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J75" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="K75" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="76">
@@ -2678,14 +2918,17 @@
         <v>0.712105619084031</v>
       </c>
       <c r="G76" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H76"/>
       <c r="I76" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J76" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="K76" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="77">
@@ -2708,14 +2951,17 @@
         <v>1.78814228178014</v>
       </c>
       <c r="G77" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H77"/>
       <c r="I77" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J77" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="K77" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="78">
@@ -2738,14 +2984,17 @@
         <v>-89.4737727014979</v>
       </c>
       <c r="G78" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H78"/>
       <c r="I78" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J78" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="K78" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="79">
@@ -2766,14 +3015,17 @@
       </c>
       <c r="F79"/>
       <c r="G79" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H79"/>
       <c r="I79" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J79" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="K79" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="80">
@@ -2796,14 +3048,17 @@
         <v>-2.14656976547731</v>
       </c>
       <c r="G80" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H80"/>
       <c r="I80" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J80" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="K80" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="81">
@@ -2824,14 +3079,17 @@
         <v>129.151953893201</v>
       </c>
       <c r="G81" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H81"/>
       <c r="I81" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J81" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="K81" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="82">
@@ -2854,14 +3112,17 @@
         <v>-1.55988622469838</v>
       </c>
       <c r="G82" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H82"/>
       <c r="I82" t="s">
+        <v>33</v>
+      </c>
+      <c r="J82" t="s">
         <v>30</v>
       </c>
-      <c r="J82" t="s">
-        <v>27</v>
+      <c r="K82" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="83">
@@ -2882,14 +3143,17 @@
         <v>90.5995528166018</v>
       </c>
       <c r="G83" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H83"/>
       <c r="I83" t="s">
+        <v>33</v>
+      </c>
+      <c r="J83" t="s">
         <v>30</v>
       </c>
-      <c r="J83" t="s">
-        <v>27</v>
+      <c r="K83" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="84">
@@ -2912,14 +3176,17 @@
         <v>-89.47377289265</v>
       </c>
       <c r="G84" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H84"/>
       <c r="I84" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J84" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="K84" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="85">
@@ -2940,14 +3207,17 @@
       </c>
       <c r="F85"/>
       <c r="G85" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H85"/>
       <c r="I85" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J85" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="K85" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="86">
@@ -2970,14 +3240,17 @@
         <v>-3.33321045341888</v>
       </c>
       <c r="G86" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H86"/>
       <c r="I86" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J86" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="K86" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="87">
@@ -3000,14 +3273,17 @@
         <v>7.57828751649767</v>
       </c>
       <c r="G87" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H87"/>
       <c r="I87" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J87" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="K87" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>